<commit_message>
update & link classes
</commit_message>
<xml_diff>
--- a/State Farm Classifier/Reviews.xlsx
+++ b/State Farm Classifier/Reviews.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Desktop\HackUTD-2021\State Farm Classifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC69C0D-82C8-4817-818F-664A6E2CE458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C35C017-B2AB-4683-933C-87DBB8FC00D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4515" yWindow="4110" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>test4</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>policy</t>
+  </si>
+  <si>
+    <t>policyType</t>
+  </si>
+  <si>
+    <t>'it just works'</t>
+  </si>
+  <si>
+    <t>'steve'</t>
+  </si>
+  <si>
+    <t>'9/10/21'</t>
+  </si>
+  <si>
+    <t>'Vehicle'</t>
+  </si>
+  <si>
+    <t>Car'</t>
+  </si>
+  <si>
+    <t>'fast service after a freak boating accident'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'gonzalez'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '3/21/17'</t>
+  </si>
+  <si>
+    <t>Vehicle'</t>
+  </si>
+  <si>
+    <t>Boat'</t>
   </si>
 </sst>
 </file>
@@ -357,15 +390,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,39 +414,48 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
         <v>3</v>
       </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
       </c>
       <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix date hour/min issue
</commit_message>
<xml_diff>
--- a/State Farm Classifier/Reviews.xlsx
+++ b/State Farm Classifier/Reviews.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Desktop\HackUTD-2021\State Farm Classifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89ECDF44-9771-4762-8F6D-A1C9004F245E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F993FE-E16E-4987-8CB1-5BDCAE74DEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4515" yWindow="4110" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Review</t>
   </si>
@@ -45,34 +45,49 @@
     <t>policyType</t>
   </si>
   <si>
-    <t>'steve'</t>
-  </si>
-  <si>
-    <t>'9/10/21'</t>
-  </si>
-  <si>
-    <t>'Vehicle'</t>
-  </si>
-  <si>
-    <t>Car'</t>
-  </si>
-  <si>
-    <t>'fast service after a freak boating accident'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'gonzalez'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> '3/21/17'</t>
-  </si>
-  <si>
-    <t>Vehicle'</t>
-  </si>
-  <si>
-    <t>Boat'</t>
-  </si>
-  <si>
-    <t>this is the worst thing I hate hate hate it</t>
+    <t>Vehicle</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>Steve Doe</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Great service, Jake was really fast and helpful and helping me with my claim</t>
+  </si>
+  <si>
+    <t>Sarah Doe</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Homeowner</t>
+  </si>
+  <si>
+    <t>I had a really unpleasant time with the new app, it was bad</t>
+  </si>
+  <si>
+    <t>Life</t>
+  </si>
+  <si>
+    <t>Whole</t>
+  </si>
+  <si>
+    <t>I love the new car policy, it was much cheaper than my previous plan</t>
+  </si>
+  <si>
+    <t>9/10/2021</t>
+  </si>
+  <si>
+    <t>3/2/2016</t>
+  </si>
+  <si>
+    <t>6/25/2011</t>
   </si>
 </sst>
 </file>
@@ -108,8 +123,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,15 +407,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -423,22 +441,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -446,22 +464,52 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>250</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update input & cleanup text formatting
</commit_message>
<xml_diff>
--- a/State Farm Classifier/Reviews.xlsx
+++ b/State Farm Classifier/Reviews.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Desktop\HackUTD-2021\State Farm Classifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F993FE-E16E-4987-8CB1-5BDCAE74DEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4A7D8B-C902-4510-BCB6-514779045E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4515" yWindow="4110" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>John Doe</t>
   </si>
   <si>
-    <t>Great service, Jake was really fast and helpful and helping me with my claim</t>
-  </si>
-  <si>
     <t>Sarah Doe</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>6/25/2011</t>
+  </si>
+  <si>
+    <t>Great service, Jake was really fast and helpful. He did an awesome job aiding me with my claim</t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,13 +441,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>45</v>
@@ -461,42 +461,42 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>100</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <v>250</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>